<commit_message>
Colocar no controlador de versão as informações dos exercícios, e o termo de privacidade
</commit_message>
<xml_diff>
--- a/DOCUMENTOS/CRONOGRAMA/Cronograma_aplicativo_integrado_com_trello.xlsx
+++ b/DOCUMENTOS/CRONOGRAMA/Cronograma_aplicativo_integrado_com_trello.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="13395" windowHeight="4680" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="13395" windowHeight="4680" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Itens iniciais" sheetId="1" r:id="rId1"/>
@@ -737,7 +737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -1148,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1249,8 +1249,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>4</v>
+      <c r="A11" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="B11" t="s">
         <v>41</v>

</xml_diff>